<commit_message>
Atualiza banco de questões (perguntascho2026.xlsx)
</commit_message>
<xml_diff>
--- a/perguntascho2026.xlsx
+++ b/perguntascho2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94D5857-BF11-4951-87BC-CDADC500EA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9651E5D-9B6D-4113-881A-3494559FA6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C9B4D97-84B9-4E48-8A8F-DF3EE0788C30}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="1441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2683" uniqueCount="1622">
   <si>
     <t>ID</t>
   </si>
@@ -8301,6 +8301,2172 @@
   </si>
   <si>
     <t>Medida protetiva</t>
+  </si>
+  <si>
+    <t>De acordo com os conceitos aplicáveis à área de abordagem a veículos definidos no MTP 04, a "Área de Aproximação" é tecnicamente descrita como:</t>
+  </si>
+  <si>
+    <t>O espaço situado dentro da área de risco onde o policial militar estará vulnerável à agressão física, compreendendo aproximadamente o raio de abertura das portas do veículo.</t>
+  </si>
+  <si>
+    <t>A área na qual a Polícia Militar tem o domínio da situação, havendo, presumidamente, menores riscos à integridade física e à segurança dos policiais militares.</t>
+  </si>
+  <si>
+    <t>O espaço que corresponde a uma faixa de aproximadamente a largura de um corpo humano, dentro da área de risco, que se inicia na altura do para-choque traseiro e termina antes do raio de abertura da porta do motorista.</t>
+  </si>
+  <si>
+    <t>O espaço destinado à realização de busca pessoal, definido após análise do local e avaliação de riscos, garantindo segurança tanto para os policiais quanto para os abordados.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A alternativa reproduz fielmente a definição contida no </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 2.2, alínea 'd'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Área de aproximação: é o espaço que corresponde a uma faixa de aproximadamente a largura de um corpo humano, dentro da área de risco, que se inicia na altura do para-choque traseiro [...] e termina antes do raio de abertura da porta do motorista...". As demais opções referem-se, respectivamente, à Área de Alcance, Área de Segurança e Área de Busca.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Na Tática de Posicionamento Diagonal com o emprego de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 (duas) viaturas e 4 (quatro) policiais militares em cada viatura</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (totalizando 8 militares), o MTP 04 estabelece um posicionamento específico para o motorista da segunda viatura e o patrulheiro que ocupava inicialmente a posição 3. Esses militares devem:</t>
+    </r>
+  </si>
+  <si>
+    <t>Permanecer no interior da segunda viatura para garantir a segurança das comunicações via rádio e consulta de dados.</t>
+  </si>
+  <si>
+    <t>Deslocar-se imediatamente para a retaguarda da segunda viatura, reforçando a segurança do perímetro juntamente com os demais patrulheiros.</t>
+  </si>
+  <si>
+    <t>Posicionar-se entre a primeira e a segunda viatura, com a arma na posição de guarda baixa e a silhueta reduzida, servindo de apoio aos policiais que ocupam as posições 1 e 2.</t>
+  </si>
+  <si>
+    <t>Ocupar a posição 4 da primeira viatura, dando cobertura direta ao Comandante da operação durante a verbalização.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 3.3.2.1, alínea 'h'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "O motorista da segunda viatura e o patrulheiro que ocupava inicialmente a posição 3 posicionar-se-ão entre a primeira e a segunda viatura, com a arma na posição de guarda baixa e a silhueta reduzida, servindo de apoio aos policiais militares que ocupam as posições 1 e 2..."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">No tocante à abordagem a caminhões de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nível 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (operações educativas ou assistenciais), o procedimento tático padrão para o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PM Verbalizador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> determina que ele deve:</t>
+    </r>
+  </si>
+  <si>
+    <t>Deslocar-se pela frente do caminhão no sentido anti-horário, mantendo contato visual constante com o motorista pela para-brisa.</t>
+  </si>
+  <si>
+    <t>Permanecer na posição 1 da viatura e utilizar o megafone para determinar que o motorista desça do veículo antes de qualquer aproximação.</t>
+  </si>
+  <si>
+    <t>Deslocar pela retaguarda do caminhão no sentido horário e realizar aproximação até aproximadamente 3 (três) a 5 (cinco) metros da cabine.</t>
+  </si>
+  <si>
+    <t>Subir no estribo do caminhão pelo lado do passageiro para garantir que não há outras pessoas na cabine antes de iniciar a verbalização.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A alternativa está correta conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.3.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "O PM Verbalizador deslocará pela retaguarda do caminhão no sentido horário e realizará aproximação até aproximadamente 3 (três) a 5 (cinco) metros da cabine, conforme Figura 38."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Durante a abordagem a um ônibus com </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 (duas) ou mais portas de acesso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> em uma operação de Nível 2, o PM Comandante deve adotar um procedimento específico quanto ao controle das portas. Segundo o manual, o procedimento CORRETO é:</t>
+    </r>
+  </si>
+  <si>
+    <t>Solicitar ao motorista que abra todas as portas simultaneamente para permitir a rápida evacuação e visualização de todos os passageiros.</t>
+  </si>
+  <si>
+    <t>Solicitar ao motorista que mantenha todas as portas fechadas até que a equipe de segurança externa esteja posicionada.</t>
+  </si>
+  <si>
+    <t>Solicitar ao motorista que abra apenas as portas dianteira e traseira e que mantenha fechada(s) a(s) porta(s) central(is), quando houver.</t>
+  </si>
+  <si>
+    <t>Determinar a abertura apenas da porta dianteira para que o PM Verbalizador entre, mantendo as demais travadas para evitar fugas.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.2.1, alínea 'b'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.2.2, alínea 'b'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Após a parada do veículo, o PM Comandante [...] solicitará ao motorista que abra apenas as portas dianteira e traseira e que mantenha fechada(s) a(s) porta(s) central(is), quando houver."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Em uma abordagem a motocicletas utilizando </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 (três) motocicletas policiais</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, o posicionamento do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PM Segurança 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> é detalhado de forma precisa. Ele deve posicionar sua motocicleta:</t>
+    </r>
+  </si>
+  <si>
+    <t>Alinhada ao PM Comandante, do lado esquerdo, para bloquear a via de trânsito em sentido contrário.</t>
+  </si>
+  <si>
+    <t>A uma distância aproximada de 1,5 (um e meio) metros à retaguarda da motocicleta do PM Comandante, na diagonal (45°), obstruindo a faixa de trânsito atrás do veículo abordado.</t>
+  </si>
+  <si>
+    <t>À frente da motocicleta abordada, a uma distância de 3 a 5 metros, impedindo a fuga do suspeito.</t>
+  </si>
+  <si>
+    <t>No passeio ou acostamento, paralelamente à motocicleta do PM Segurança 1, para realizar a segurança periférica.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A alternativa respeita a literalidade do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 3.4.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "O PM Segurança 2 posicionará a motocicleta a uma distância aproximada de 1,5 (um e meio) metros à retaguarda da motocicleta do PM Comandante, na diagonal (45°) obstruindo a faixa de trânsito atrás do veículo abordado."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Na montagem do dispositivo de bloqueio na via (Operação Cerco e Bloqueio), o MTP 04 estabelece a criação de três barreiras distintas. A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>terceira barreira</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> é caracterizada:</t>
+    </r>
+  </si>
+  <si>
+    <t>Pela disposição de cones distribuídos ao longo da pista para canalizar o trânsito.</t>
+  </si>
+  <si>
+    <t>Pela colocação de cavaletes com a indicação de bloqueio da pista.</t>
+  </si>
+  <si>
+    <t>Pela disposição das viaturas na via, posicionadas num ângulo de 45° com a frente voltada para o sentido da via.</t>
+  </si>
+  <si>
+    <t>Pelo posicionamento dos policiais militares com armas longas e escudos balísticos.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subitem 5.5.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "3ª barreira: concretizada pela disposição das viaturas na via [...] a viatura ficará posicionada num ângulo de 45°, com a frente voltada para o sentido da via...". A 1ª barreira são cavaletes e a 2ª são cones.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Quanto ao emprego de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>limitadores de fuga</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (como a "cama de faquir") em uma operação de bloqueio, o manual determina que o equipamento deve ser instalado em uma posição específica relativa às barreiras montadas. A posição correta é:</t>
+    </r>
+  </si>
+  <si>
+    <t>Imediatamente antes da primeira barreira, para surpreender o condutor antes que ele visualize o bloqueio.</t>
+  </si>
+  <si>
+    <t>Entre a primeira e a segunda barreira, a uma distância de 10 metros da primeira.</t>
+  </si>
+  <si>
+    <t>Exatamente na linha da terceira barreira, protegido pelas viaturas policiais.</t>
+  </si>
+  <si>
+    <t>Entre a segunda e a terceira barreira de contenção, a 5 (cinco) metros de distância da segunda barreira.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A alternativa está correta baseada no </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subitem 6.2.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "...o limitador de fuga deve ser instalado entre a segunda e a terceira barreira de contenção, a 5 (cinco) metros de distância da segunda barreira."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Durante a realização de uma perseguição policial (intervenção de nível III), o MTP 04 lista medidas que o policial militar </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NÃO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> deve executar devido aos riscos envolvidos. Dentre essas vedações expressas, encontra-se:</t>
+    </r>
+  </si>
+  <si>
+    <t>Utilizar sinais luminosos e sirene para sinalizar a situação de emergência.</t>
+  </si>
+  <si>
+    <t>Manter a distância mínima de segurança da viatura em relação ao veículo em fuga.</t>
+  </si>
+  <si>
+    <t>Ultrapassar ou emparelhar a viatura com o veículo em fuga, efetuando manobras perigosas ("fechadas").</t>
+  </si>
+  <si>
+    <t>Repassar ao COPOM dados do veículo em fuga, como tipo, marca, modelo e placa.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 5.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04 (página 80), recomenda-se ao policial militar que não execute: "ultrapassar ou emparelhar a viatura com o veículo em fuga, efetuando manobras perigosas ('fechadas')". As demais opções são procedimentos recomendados nas alíneas 'b', 'c' e 'e'.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sobre a busca em ônibus, o MTP 04 identifica diversos locais utilizados para ocultação de ilícitos. Sobre a conferência de bagagens no bagageiro externo de ônibus interestaduais e intermunicipais, o procedimento descrito é:</t>
+  </si>
+  <si>
+    <t>A busca deve ser feita exclusivamente pelos passageiros proprietários das malas, sob supervisão visual do policial, sendo vedado o toque do militar na bagagem.</t>
+  </si>
+  <si>
+    <t>O Auxiliar de viagem ou motorista do ônibus poderá ser acionado para a conferência da etiqueta de identificação da bagagem e será arrolado como testemunha da ação policial.</t>
+  </si>
+  <si>
+    <t>As malas devem ser retiradas e colocadas na pista de rolamento para que cães farejadores realizem a inspeção inicial, dispensando a presença do motorista.</t>
+  </si>
+  <si>
+    <t>O policial deve abrir todas as malas imediatamente, independentemente da identificação do proprietário, para garantir a rapidez da operação (princípio da celeridade).</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.2.1, alínea 'a'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (final do tópico) e </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.4, alínea 'i'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "O Auxiliar de viagem ou motorista do ônibus poderá ser acionado para a conferência da etiqueta de identificação da bagagem e será arrolado como testemunha da ação policial."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Na </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tática de Posicionamento Diagonal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para abordagem a veículos de passeio (nível 2 ou 3), o MTP 04 estabelece que, ao iniciarem a verbalização para desembarque, os policiais devem determinar que o motorista abra a porta traseira do veículo. O procedimento correto descrito é:</t>
+    </r>
+  </si>
+  <si>
+    <t>O motorista deve abrir a porta traseira utilizando a mão direita, mantendo a esquerda no volante.</t>
+  </si>
+  <si>
+    <t>O motorista deve descer do veículo, abrir a porta traseira por fora e retornar ao volante.</t>
+  </si>
+  <si>
+    <t>O motorista deve abrir a porta traseira do seu veículo com a mão esquerda (as portas permanecem abertas).</t>
+  </si>
+  <si>
+    <t>O motorista não deve abrir a porta traseira; esta ação deve ser realizada exclusivamente pelo PM Vistoriador após a contenção dos ocupantes.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme a verbalização sugerida no </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 3.3.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Com a mão esquerda, abra a porta traseira do seu veículo! (as portas permanecem abertas)."</t>
+    </r>
+  </si>
+  <si>
+    <t>MTP - 04</t>
+  </si>
+  <si>
+    <t>Conforme as Considerações Iniciais do MTP 04, acerca da necessidade de mandado judicial para a realização de busca em veículos, é CORRETO afirmar que:</t>
+  </si>
+  <si>
+    <t>A busca veicular sempre dependerá de mandado judicial, exceto quando o veículo estiver em movimento, situação que configura flagrante ficto.</t>
+  </si>
+  <si>
+    <t>A busca veicular independerá de mandado, visto que o Art. 244 do CPP descreve que a busca pessoal independe de mandado e o veículo, quando não utilizado como moradia, não goza da proteção de inviolabilidade domiciliar.</t>
+  </si>
+  <si>
+    <t>A busca veicular exige mandado judicial apenas para a vistoria de compartimentos fechados, como porta-malas e porta-luvas, sendo dispensada para a área de passageiros.</t>
+  </si>
+  <si>
+    <t>A busca veicular independe de mandado judicial apenas se o condutor autorizar expressamente a medida, devendo tal consentimento ser registrado em vídeo ou por escrito.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 2 (Considerações Iniciais)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04 (pág. 14): "O art. 244 do CPP descreve que a busca pessoal independerá de mandado, e o art. 245 condiciona a necessidade de mandado apenas para a busca domiciliar. Portanto, nos veículos em que o proprietário/condutor não utiliza como moradia, a busca pessoal e a vistoria veicular independem da necessidade de mandado."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O MTP 04 estabelece uma distinção técnica precisa entre os conceitos de "Busca Veicular" e "Vistoria". Assinale a alternativa que define corretamente a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vistoria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, segundo a literalidade do manual:</t>
+    </r>
+  </si>
+  <si>
+    <t>Consiste na verificação interna e externa do veículo abordado, por meio de revista nos compartimentos suscetíveis a serem utilizados para esconder objetos ilícitos.</t>
+  </si>
+  <si>
+    <t>É o procedimento de identificação criminal dos ocupantes do veículo através de consulta aos sistemas informatizados de segurança pública.</t>
+  </si>
+  <si>
+    <t>Consiste no processo de conferência do chassi, número do motor, carrocerias, placas e outros sinais veiculares, verificando se estão dentro das especificações exigidas pelas normas de trânsito.</t>
+  </si>
+  <si>
+    <t>É a varredura visual realizada pelo policial militar da posição 1 (Verbalizador) antes de autorizar o desembarque dos ocupantes do veículo.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A alternativa reproduz fielmente o conceito do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 3.3.2.2, alínea 'b'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Vistoria: consiste no processo de conferência do chassi, número do motor, carrocerias, placas e outros sinais veiculares, verificando se estão dentro das especificações exigidas pelas normas de trânsito." A opção A define "Busca Veicular".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Durante a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Abordagem a Ônibus Nível 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (preventiva) em um veículo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sem roleta e com uma porta de acesso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, o MTP 04 determina um posicionamento específico para o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PM Revistador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (terceiro policial). Este deve posicionar-se:</t>
+    </r>
+  </si>
+  <si>
+    <t>Próximo à parte central do ônibus sobre o passeio/acostamento com as atenções voltadas para o interior do coletivo.</t>
+  </si>
+  <si>
+    <t>Sobre a calçada/acostamento, próximo a parte traseira do coletivo, assumindo a função de segurança externa.</t>
+  </si>
+  <si>
+    <t>No interior do ônibus, deslocando-se imediatamente para o fundo do corredor para realizar a varredura visual.</t>
+  </si>
+  <si>
+    <t>Junto à porta dianteira, ao lado do PM Comandante, para auxiliar na verbalização com o motorista.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.2.1, alínea 'a'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "O terceiro policial militar que assumirá a função de PM Revistador posicionar-se-á próximo à parte central do ônibus sobre o passeio/acostamento com as atenções voltadas para o interior do coletivo."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nas abordagens a caminhões de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Níveis 2 e 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (preventiva com suspeita ou repressiva), os procedimentos táticos seguem a Tática de Posicionamento Diagonal, porém com uma adaptação específica para o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PM Comandante/Segurança</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Segundo o manual, este policial deve posicionar-se:</t>
+    </r>
+  </si>
+  <si>
+    <t>À frente da cabine do caminhão, utilizando a viatura como abrigo para monitorar o motorista.</t>
+  </si>
+  <si>
+    <t>Alinhado e junto à extremidade traseira direita do caminhão.</t>
+  </si>
+  <si>
+    <t>Na posição 4, dando cobertura ao PM Verbalizador, que se encontra na escada de acesso à cabine.</t>
+  </si>
+  <si>
+    <t>Sobre o estribo do lado do passageiro para garantir a visualização interna da cabine.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.3.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Os procedimentos táticos devem seguir o descrito na subseção 3.3.2 (Tática de posicionamento Diagonal), devendo adaptar o posicionamento do PM Comandante/Segurança que se posicionará alinhado e junto à extremidade traseira direita do caminhão."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Na montagem do dispositivo de cerco da via, o MTP 04 descreve o tipo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Afunilamento Diagonal"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Nesta configuração, os cones devem ser dispostos:</t>
+    </r>
+  </si>
+  <si>
+    <t>Formando um "zigue-zague" na via, obrigando o veículo a reduzir a velocidade drasticamente.</t>
+  </si>
+  <si>
+    <t>Longitudinalmente na mesma faixa em que a viatura estiver posicionada (paralelo ao fluxo).</t>
+  </si>
+  <si>
+    <t>Na mesma faixa em que a viatura estiver posicionada, formando um fluxo diagonal.</t>
+  </si>
+  <si>
+    <t>Transversalmente à via, bloqueando totalmente todas as faixas de rolamento.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 5.4.1, alínea 'c'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Afunilamento Diagonal: [...] Os cones serão dispostos na mesma faixa em que a viatura estiver posicionada, formando um fluxo diagonal, conforme a Figura 42."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O MTP 04 lista diversos locais utilizados para ocultação de ilícitos em ônibus. Sobre a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>caixa de fusíveis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, o manual especifica que este compartimento situa-se, costumeiramente:</t>
+    </r>
+  </si>
+  <si>
+    <t>No compartimento do motor, acessível apenas pela parte externa.</t>
+  </si>
+  <si>
+    <t>Ao lado esquerdo do assento do motorista, na parte superior.</t>
+  </si>
+  <si>
+    <t>Abaixo do painel principal, próximo aos pedais de comando.</t>
+  </si>
+  <si>
+    <t>No teto do veículo, junto ao letreiro luminoso.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.4, alínea 'f'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "caixa de fusíveis: situada, costumeiramente, ao lado esquerdo do assento do motorista, na parte superior. Também permite o esconderijo de objetos de diversos tamanhos."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segundo a fundamentação legal apresentada no MTP 04 sobre a perseguição policial, o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Flagrante Impróprio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (ou quase flagrância), previsto no inciso III do art. 302 do CPP, ocorre quando o agente:</t>
+    </r>
+  </si>
+  <si>
+    <t>É encontrado, logo depois, com instrumentos, armas, objetos ou papéis que façam presumir ser ele autor da infração.</t>
+  </si>
+  <si>
+    <t>Está cometendo a infração penal ou acaba de cometê-la.</t>
+  </si>
+  <si>
+    <t>É perseguido, logo após, pela autoridade, pelo ofendido ou por qualquer pessoa, em situação que faça presumir ser autor da infração.</t>
+  </si>
+  <si>
+    <t>Confessa a autoria do delito espontaneamente ao ser abordado pela autoridade policial.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 5.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04, que cita o Art. 302 do CPP: "III - é perseguido, logo após, pela autoridade, pelo ofendido ou por qualquer pessoa, em situação que faça presumir ser autor da infração." (A opção A refere-se ao flagrante presumido/ficto, inciso IV).</t>
+    </r>
+  </si>
+  <si>
+    <t>Sobre as limitações no uso dos limitadores de fuga (ex: "cama de faquir"), o MTP 04 alerta que o esvaziamento dos pneus pode não ocorrer tão rápido quanto se espera em virtude de:</t>
+  </si>
+  <si>
+    <t>O pneu do veículo conter fluídos que blindam sua "banda de rodagem".</t>
+  </si>
+  <si>
+    <t>A temperatura do asfalto dilatar a borracha do pneu, vedando os furos instantaneamente.</t>
+  </si>
+  <si>
+    <t>O peso do veículo ser insuficiente para pressionar as agulhas da base pantográfica.</t>
+  </si>
+  <si>
+    <t>As agulhas serem projetadas apenas para pneus de veículos de carga, não sendo eficazes em veículos de passeio.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 6.5, alínea 'a'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "no emprego do limitador de fuga, tipo 'cama de faquir', em virtude do pneu do veículo conter fluídos que blindam sua 'banda de rodagem', o esvaziamento pode não ocorrer tão rápido quanto se espera."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O MTP 04 descreve um tipo de limitador de fuga conhecido como </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"bollards"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ou "cabeços". Sobre este equipamento, o manual afirma que são:</t>
+    </r>
+  </si>
+  <si>
+    <t>Dispositivos móveis constituídos de agulhas de aço distribuídos numa base pantográfica.</t>
+  </si>
+  <si>
+    <t>Postes de amarração que podem ser colocados com a finalidade de evitar a passagem de veículos em todos os momentos ou somente em determinados horários.</t>
+  </si>
+  <si>
+    <t>Barras de ferro com pontas, lançadas manualmente sob as rodas do veículo em movimento.</t>
+  </si>
+  <si>
+    <t>Redes de contenção utilizadas para envolver o veículo e travar o eixo motriz.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 6.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Existem limitadores que são postes/pilares móveis, também conhecidos como 'bollards', ou 'cabeços', ou ainda, 'postes de amarração que podem ser colocados com a finalidade de evitar a passagem de veículos em todos os momentos ou somente em determinados horários..."</t>
+    </r>
+  </si>
+  <si>
+    <t>Durante a abordagem a ônibus, no tocante aos pertences pessoais, o MTP 04 orienta que, caso o policial militar se depare com objetos relativos à intimidade do abordado que, se expostos, causarão constrangimentos, e não havendo nada de ilegal, deve-se:</t>
+  </si>
+  <si>
+    <t>Apreender os objetos preventivamente para evitar reclamações futuras na Corregedoria.</t>
+  </si>
+  <si>
+    <t>Devolver a bolsa e agir com profissionalismo e discrição, atentando para o fato de que o abordado seguirá no coletivo.</t>
+  </si>
+  <si>
+    <t>Mostrar os objetos ao motorista do ônibus para que este sirva de testemunha da lisura da ação policial.</t>
+  </si>
+  <si>
+    <t>Solicitar que o abordado desça do ônibus com seus pertences e aguarde a próxima condução, para evitar o contato com os demais passageiros.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.2.1 (verbalização)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04 (pág. 57): "Pode ser que o policial militar se depare com alguns objetos relativos à intimidade do abordado que, se expostos, causarão constrangimentos. [...] caso não encontre objeto ilícito, devolva a bolsa. [...] Por isso, aja com profissionalismo e discrição."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Durante o patrulhamento, a Guarnição do Sgt Lopes recebe uma denúncia anônima de que há um veículo parado em frente a um estabelecimento comercial há muito tempo, causando suspeição aos comerciantes locais, embora não haja visualização de armas. Com base na classificação de risco apresentada no MTP 04, qual é o nível de abordagem, o risco e o estado de prontidão coerente que a equipe deve adotar?</t>
+    </r>
+  </si>
+  <si>
+    <t>Nível 1; Risco I (Educativo); Estado de Prontidão Atenção (Amarelo).</t>
+  </si>
+  <si>
+    <t>Nível 2; Risco II (Preventiva/Fundada Suspeita); Estado de Prontidão Alerta (Laranja).</t>
+  </si>
+  <si>
+    <t>Nível 3; Risco III (Repressiva); Estado de Prontidão Alarme (Vermelho).</t>
+  </si>
+  <si>
+    <t>Nível 2; Risco III (Repressiva); Estado de Prontidão Alarme (Vermelho), devido à denúncia.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 2.1, alínea 'b'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Abordagem a veículo - nível 2: Será empregada nas ações e operações de verificação preventiva (risco nível II) [...] É o caso das [...] denúncia de veículos em locais ermos ou parados em frente a estabelecimentos comerciais, causando suspeição de comerciantes [...] O estado de prontidão coerente é o alerta (laranja)."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A equipe do Cabo Valente realiza uma abordagem diagonal a um veículo com vidros escuros. Após o desembarque de todos os ocupantes visíveis, o Cb Valente (PM Verbalizador), ao realizar a varredura visual aproximando-se pelo lado esquerdo, identifica um passageiro escondido deitado no banco traseiro.Diante dessa situação, qual a conduta imediata preconizada pelo manual?</t>
+    </r>
+  </si>
+  <si>
+    <t>O policial deve quebrar o vidro lateral com o bastão para garantir a entrada dinâmica e render o suspeito imediatamente.</t>
+  </si>
+  <si>
+    <t>O policial deve abrir a porta bruscamente e ordenar que o passageiro saia, mantendo a arma em posição de tiro.</t>
+  </si>
+  <si>
+    <t>A equipe deverá executar o recuo tático e iniciar um novo processo de verbalização na área de segurança.</t>
+  </si>
+  <si>
+    <t>O PM Segurança deve disparar um tiro de advertência para compelir o passageiro a se entregar.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 3.3.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04 (pág. 32): "Caso identifiquem a presença de passageiro escondido no interior do veículo, deverão executar o recuo tático e iniciar um novo processo de verbalização na área de segurança."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Uma guarnição Tático Móvel depara-se com um ônibus onde passageiros sinalizam que está ocorrendo um assalto à mão armada (Nível 3). A viatura realiza a parada do coletivo.Considerando as dimensões do veículo e a necessidade de segurança, qual a distância e o posicionamento correto da viatura em relação ao ônibus?</t>
+    </r>
+  </si>
+  <si>
+    <t>A viatura deve posicionar-se à frente do ônibus para bloquear o deslocamento, a uma distância de 2 metros.</t>
+  </si>
+  <si>
+    <t>A viatura deve emparelhar com a porta dianteira para permitir a entrada rápida da equipe de assalto.</t>
+  </si>
+  <si>
+    <t>A guarnição posicionará sua viatura atrás do ônibus, a uma distância de 5 (cinco) a 10 (dez) metros, na diagonal em relação à via.</t>
+  </si>
+  <si>
+    <t>A guarnição deve posicionar a viatura a 20 metros de distância, totalmente alinhada (paralela) à traseira do ônibus para usar o motor como blindagem.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A alternativa reproduz o procedimento do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Nesse sentido, após a parada efetiva do ônibus, a guarnição policial posicionará sua viatura atrás dele, a uma distância de 5 (cinco) a 10 (dez) metros, na diagonal em relação à via."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> O Sargento P. Silva comanda uma operação de Blitz e decide abordar um caminhão baú para fiscalização de rotina (Nível 1). Ao determinar as posições, ele ordena que o PM Segurança monitore a cabine.Segundo o MTP 04, qual o posicionamento específico do PM Segurança nesta modalidade (Nível 1)?</t>
+    </r>
+  </si>
+  <si>
+    <t>Deve posicionar-se próximo à viatura policial ou outro abrigo existente no ambiente à frente do caminhão.</t>
+  </si>
+  <si>
+    <t>Deve subir no estribo do lado do motorista para garantir que ele desligue o veículo.</t>
+  </si>
+  <si>
+    <t>Deve posicionar-se na retaguarda do caminhão, garantindo a segurança do perímetro traseiro.</t>
+  </si>
+  <si>
+    <t>Deve ficar alinhado à porta do passageiro para realizar a varredura visual simultânea.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.3.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "O PM Segurança posicionará próximo à viatura policial ou outro abrigo existente no ambiente à frente do caminhão, de forma a monitorar o interior da cabine até o PM Verbalizador ter condições de verbalizar com o motorista."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Durante uma busca minuciosa em um ônibus intermunicipal suspeito de tráfico, o Sd Novato encontra um compartimento falso próximo ao motorista, especificamente na "mesa do trocador/caixa". O motorista alega que a polícia não pode revistar ali por ser responsabilidade da empresa.Com base no MTP 04, a suspeita do policial é tecnicamente fundamentada pois:</t>
+    </r>
+  </si>
+  <si>
+    <t>O manual descreve que os infratores costumam obrigar o funcionário a esconder ilícitos na mesa do trocador, acreditando que não será alvo de fiscalização.</t>
+  </si>
+  <si>
+    <t>O manual proíbe a revista na mesa do trocador, salvo com mandado judicial específico para a empresa de transporte.</t>
+  </si>
+  <si>
+    <t>A mesa do trocador é o único local onde não se pode esconder armas longas, apenas drogas.</t>
+  </si>
+  <si>
+    <t>O manual orienta que a revista nesse local deve ser feita apenas pela Polícia Rodoviária Federal.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 4.2.4, alínea 'c'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "mesa do trocador/caixa: [...] Os infratores costumam [...] obrigar o funcionário a esconder armas, drogas e outros objetos, acreditando que, por ser o local de responsabilidade dos profissionais do transporte, não será alvo da fiscalização policial."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> O Tenente R. Alves está coordenando uma perseguição policial via rádio. Ele insiste rigorosamente na disciplina de comunicações, impedindo conversas paralelas.Segundo o MTP 04, além de fazer as ordens alcançarem todos os envolvidos, quais são as outras DUAS razões essenciais listadas para essa disciplina de rádio?</t>
+    </r>
+  </si>
+  <si>
+    <t>Garantir a gravação para fins judiciais e permitir que a imprensa acompanhe a ocorrência em tempo real.</t>
+  </si>
+  <si>
+    <t>Auxiliar no controle do nível de estresse da ocorrência e impedir que mensagens confusas alterem o estado de prontidão dos policiais militares.</t>
+  </si>
+  <si>
+    <t>Evitar o congestionamento da rede para outras ocorrências e permitir que o Comandante Geral ouça a operação.</t>
+  </si>
+  <si>
+    <t>Garantir que o infrator não ouça a estratégia policial (caso tenha rádio na frequência) e economizar bateria dos HTs.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 5.3 (Lembre-se)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04: "Três razões essenciais para a disciplina das comunicações na rede-rádio: a) fazer com que as ordens [...] alcancem todos os envolvidos; b) auxiliar no controle do nível de estresse da ocorrência; c) impedir que mensagens confusas alterem o estado de prontidão dos policiais militares."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Um veículo em alta velocidade fura o bloqueio policial montado pela equipe do Sgt Peixoto, sem autorização, colocando em risco a guarnição.À luz da fundamentação legal citada no MTP 04 (Art. 210 do CTB), essa conduta de "transpor, sem autorização, bloqueio viário policial" classifica-se como:</t>
+    </r>
+  </si>
+  <si>
+    <t>Infração Grave.</t>
+  </si>
+  <si>
+    <t>Infração Média, sujeita a multa.</t>
+  </si>
+  <si>
+    <t>Infração Gravíssima.</t>
+  </si>
+  <si>
+    <t>Crime de Trânsito inafiançável.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 5.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04, que cita o CTB: "Art. 210. Transpor, sem autorização, bloqueio viário policial; Infração - gravíssima". (Diferente do Art. 209 que é transpor bloqueio sem sinalização policial, que é Grave).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A guarnição realiza uma abordagem a um veículo suspeito em uma estrada rural com </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>baixa luminosidade</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.Qual recurso o MTP 04 recomenda utilizar especificamente nessa condição para obter vantagem tática sobre o abordado?</t>
+    </r>
+  </si>
+  <si>
+    <t>O farol alto da viatura ligado intermitentemente.</t>
+  </si>
+  <si>
+    <t>A utilização da lanterna como recurso para ofuscamento da visão do abordado.</t>
+  </si>
+  <si>
+    <t>O uso de granadas de efeito moral para atordoamento prévio.</t>
+  </si>
+  <si>
+    <t>O uso de visão noturna acoplada ao armamento.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 3.3.2.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04 (pág. 43): "Em casos de abordagens com baixa luminosidade, recomenda-se a utilização da lanterna como recurso para ofuscamento da visão do abordado."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A equipe do Cb Mendes está posicionada em um bloqueio. De repente, um veículo suspeito (que não está sendo perseguido por nenhuma viatura) entra na área do bloqueio e para diante dos obstáculos.Qual o procedimento correto a ser adotado pela equipe do bloqueio segundo o MTP 04?</t>
+    </r>
+  </si>
+  <si>
+    <t>Aguardar a chegada de uma viatura de perseguição para realizar a abordagem.</t>
+  </si>
+  <si>
+    <t>Ordenar que o motorista jogue a chave pela janela e aguardar 10 minutos.</t>
+  </si>
+  <si>
+    <t>Realizar a interceptação dentro das condições existentes, realizando a progressão tática e seguindo as orientações com relação a abordagem a veículos.</t>
+  </si>
+  <si>
+    <t>Disparar nos pneus para garantir a imobilização total antes de qualquer aproximação.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 5.5.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04 (pág. 86): "Caso o veículo em fuga adentre ao bloqueio e não esteja sendo perseguido, os policiais empregados no bloqueio devem realizar a interceptação dentro das condições existentes, realizando a progressão tática e seguindo as orientações com relação a abordagem a veículos descritas neste manual."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SITUAÇÃO HIPOTÉTICA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Uma guarnição da PMMG inicia uma perseguição a um infrator em Belo Horizonte. A perseguição é contínua e ininterrupta, e o infrator é alcançado e preso apenas na cidade de Contagem (outra comarca).Baseado no Art. 290 do CPP citado no manual, qual o procedimento legal correto quanto à apresentação do preso?</t>
+    </r>
+  </si>
+  <si>
+    <t>O executor deve retornar a Belo Horizonte e apresentar o preso à autoridade do local onde o crime se originou.</t>
+  </si>
+  <si>
+    <t>O executor deve efetuar a prisão no lugar onde o alcançar, apresentando-o imediatamente à autoridade local (Contagem).</t>
+  </si>
+  <si>
+    <t>A prisão é ilegal, pois a guarnição perdeu a jurisdição ao cruzar o limite do município.</t>
+  </si>
+  <si>
+    <t>O executor deve aguardar a chegada da Polícia Militar de Contagem para que esta efetue a prisão formalmente.</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPLICAÇÃO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Conforme o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item 5.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do MTP 04, citando o Art. 290 do CPP: "Se o réu, sendo perseguido, passar ao território de outro município ou comarca, o executor poderá efetuar-lhe a prisão no lugar onde o alcançar, apresentando-o imediatamente à autoridade local..."</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -8401,7 +10567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8420,6 +10586,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8755,10 +10927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA53096D-6A57-4F0C-A4DE-F244F8C28EE1}">
-  <dimension ref="A1:M238"/>
+  <dimension ref="A1:M268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150:A238"/>
+    <sheetView tabSelected="1" topLeftCell="H254" workbookViewId="0">
+      <selection activeCell="J269" sqref="J269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.5703125" defaultRowHeight="15"/>
@@ -17149,6 +19321,1056 @@
         <v>1383</v>
       </c>
     </row>
+    <row r="239" spans="1:11" ht="45">
+      <c r="A239" s="3">
+        <v>238</v>
+      </c>
+      <c r="B239" t="s">
+        <v>12</v>
+      </c>
+      <c r="C239" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D239" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E239" s="7" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F239" s="7" t="s">
+        <v>1442</v>
+      </c>
+      <c r="G239" s="7" t="s">
+        <v>1443</v>
+      </c>
+      <c r="H239" s="7" t="s">
+        <v>1444</v>
+      </c>
+      <c r="I239" s="7" t="s">
+        <v>1445</v>
+      </c>
+      <c r="J239" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K239" s="8" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" ht="45">
+      <c r="A240" s="3">
+        <v>239</v>
+      </c>
+      <c r="B240" t="s">
+        <v>12</v>
+      </c>
+      <c r="C240" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D240" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E240" s="7" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F240" s="7" t="s">
+        <v>1448</v>
+      </c>
+      <c r="G240" s="7" t="s">
+        <v>1449</v>
+      </c>
+      <c r="H240" s="7" t="s">
+        <v>1450</v>
+      </c>
+      <c r="I240" s="7" t="s">
+        <v>1451</v>
+      </c>
+      <c r="J240" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K240" s="8" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" ht="30">
+      <c r="A241" s="3">
+        <v>240</v>
+      </c>
+      <c r="B241" t="s">
+        <v>12</v>
+      </c>
+      <c r="C241" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D241" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E241" s="7" t="s">
+        <v>1453</v>
+      </c>
+      <c r="F241" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="G241" s="7" t="s">
+        <v>1455</v>
+      </c>
+      <c r="H241" s="7" t="s">
+        <v>1456</v>
+      </c>
+      <c r="I241" s="7" t="s">
+        <v>1457</v>
+      </c>
+      <c r="J241" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K241" s="8" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" ht="30">
+      <c r="A242" s="3">
+        <v>241</v>
+      </c>
+      <c r="B242" t="s">
+        <v>12</v>
+      </c>
+      <c r="C242" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D242" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E242" s="7" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F242" s="7" t="s">
+        <v>1460</v>
+      </c>
+      <c r="G242" s="7" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H242" s="7" t="s">
+        <v>1462</v>
+      </c>
+      <c r="I242" s="7" t="s">
+        <v>1463</v>
+      </c>
+      <c r="J242" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K242" s="8" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" ht="30">
+      <c r="A243" s="3">
+        <v>242</v>
+      </c>
+      <c r="B243" t="s">
+        <v>12</v>
+      </c>
+      <c r="C243" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D243" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E243" s="7" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F243" s="7" t="s">
+        <v>1466</v>
+      </c>
+      <c r="G243" s="7" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H243" s="7" t="s">
+        <v>1468</v>
+      </c>
+      <c r="I243" s="7" t="s">
+        <v>1469</v>
+      </c>
+      <c r="J243" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K243" s="8" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" ht="30">
+      <c r="A244" s="3">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>12</v>
+      </c>
+      <c r="C244" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D244" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E244" s="7" t="s">
+        <v>1471</v>
+      </c>
+      <c r="F244" s="7" t="s">
+        <v>1472</v>
+      </c>
+      <c r="G244" s="7" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H244" s="7" t="s">
+        <v>1474</v>
+      </c>
+      <c r="I244" s="7" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J244" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K244" s="8" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" ht="30">
+      <c r="A245" s="3">
+        <v>244</v>
+      </c>
+      <c r="B245" t="s">
+        <v>12</v>
+      </c>
+      <c r="C245" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D245" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E245" s="7" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F245" s="7" t="s">
+        <v>1478</v>
+      </c>
+      <c r="G245" s="7" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H245" s="7" t="s">
+        <v>1480</v>
+      </c>
+      <c r="I245" s="7" t="s">
+        <v>1481</v>
+      </c>
+      <c r="J245" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K245" s="8" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" ht="30">
+      <c r="A246" s="3">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
+        <v>12</v>
+      </c>
+      <c r="C246" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D246" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E246" s="7" t="s">
+        <v>1483</v>
+      </c>
+      <c r="F246" s="7" t="s">
+        <v>1484</v>
+      </c>
+      <c r="G246" s="7" t="s">
+        <v>1485</v>
+      </c>
+      <c r="H246" s="7" t="s">
+        <v>1486</v>
+      </c>
+      <c r="I246" s="7" t="s">
+        <v>1487</v>
+      </c>
+      <c r="J246" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K246" s="8" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" ht="30">
+      <c r="A247" s="3">
+        <v>246</v>
+      </c>
+      <c r="B247" t="s">
+        <v>12</v>
+      </c>
+      <c r="C247" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D247" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E247" s="7" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F247" s="7" t="s">
+        <v>1490</v>
+      </c>
+      <c r="G247" s="7" t="s">
+        <v>1491</v>
+      </c>
+      <c r="H247" s="7" t="s">
+        <v>1492</v>
+      </c>
+      <c r="I247" s="7" t="s">
+        <v>1493</v>
+      </c>
+      <c r="J247" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K247" s="8" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" ht="30">
+      <c r="A248" s="3">
+        <v>247</v>
+      </c>
+      <c r="B248" t="s">
+        <v>12</v>
+      </c>
+      <c r="C248" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D248" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E248" s="7" t="s">
+        <v>1495</v>
+      </c>
+      <c r="F248" s="7" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G248" s="7" t="s">
+        <v>1497</v>
+      </c>
+      <c r="H248" s="7" t="s">
+        <v>1498</v>
+      </c>
+      <c r="I248" s="7" t="s">
+        <v>1499</v>
+      </c>
+      <c r="J248" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K248" s="8" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" ht="45">
+      <c r="A249" s="3">
+        <v>248</v>
+      </c>
+      <c r="B249" t="s">
+        <v>12</v>
+      </c>
+      <c r="C249" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D249" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E249" s="7" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F249" s="7" t="s">
+        <v>1503</v>
+      </c>
+      <c r="G249" s="7" t="s">
+        <v>1504</v>
+      </c>
+      <c r="H249" s="7" t="s">
+        <v>1505</v>
+      </c>
+      <c r="I249" s="7" t="s">
+        <v>1506</v>
+      </c>
+      <c r="J249" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K249" s="8" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" ht="30">
+      <c r="A250" s="3">
+        <v>249</v>
+      </c>
+      <c r="B250" t="s">
+        <v>12</v>
+      </c>
+      <c r="C250" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D250" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E250" s="7" t="s">
+        <v>1508</v>
+      </c>
+      <c r="F250" s="7" t="s">
+        <v>1509</v>
+      </c>
+      <c r="G250" s="7" t="s">
+        <v>1510</v>
+      </c>
+      <c r="H250" s="7" t="s">
+        <v>1511</v>
+      </c>
+      <c r="I250" s="7" t="s">
+        <v>1512</v>
+      </c>
+      <c r="J250" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K250" s="8" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" ht="30">
+      <c r="A251" s="3">
+        <v>250</v>
+      </c>
+      <c r="B251" t="s">
+        <v>12</v>
+      </c>
+      <c r="C251" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D251" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E251" s="7" t="s">
+        <v>1514</v>
+      </c>
+      <c r="F251" s="7" t="s">
+        <v>1515</v>
+      </c>
+      <c r="G251" s="7" t="s">
+        <v>1516</v>
+      </c>
+      <c r="H251" s="7" t="s">
+        <v>1517</v>
+      </c>
+      <c r="I251" s="7" t="s">
+        <v>1518</v>
+      </c>
+      <c r="J251" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K251" s="8" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" ht="45">
+      <c r="A252" s="3">
+        <v>251</v>
+      </c>
+      <c r="B252" t="s">
+        <v>12</v>
+      </c>
+      <c r="C252" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D252" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E252" s="7" t="s">
+        <v>1520</v>
+      </c>
+      <c r="F252" s="7" t="s">
+        <v>1521</v>
+      </c>
+      <c r="G252" s="7" t="s">
+        <v>1522</v>
+      </c>
+      <c r="H252" s="7" t="s">
+        <v>1523</v>
+      </c>
+      <c r="I252" s="7" t="s">
+        <v>1524</v>
+      </c>
+      <c r="J252" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K252" s="8" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" ht="30">
+      <c r="A253" s="3">
+        <v>252</v>
+      </c>
+      <c r="B253" t="s">
+        <v>12</v>
+      </c>
+      <c r="C253" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D253" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E253" s="7" t="s">
+        <v>1526</v>
+      </c>
+      <c r="F253" s="7" t="s">
+        <v>1527</v>
+      </c>
+      <c r="G253" s="7" t="s">
+        <v>1528</v>
+      </c>
+      <c r="H253" s="7" t="s">
+        <v>1529</v>
+      </c>
+      <c r="I253" s="7" t="s">
+        <v>1530</v>
+      </c>
+      <c r="J253" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K253" s="8" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" ht="30">
+      <c r="A254" s="3">
+        <v>253</v>
+      </c>
+      <c r="B254" t="s">
+        <v>12</v>
+      </c>
+      <c r="C254" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D254" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E254" s="7" t="s">
+        <v>1532</v>
+      </c>
+      <c r="F254" s="7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="G254" s="7" t="s">
+        <v>1534</v>
+      </c>
+      <c r="H254" s="7" t="s">
+        <v>1535</v>
+      </c>
+      <c r="I254" s="7" t="s">
+        <v>1536</v>
+      </c>
+      <c r="J254" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K254" s="8" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" ht="30">
+      <c r="A255" s="3">
+        <v>254</v>
+      </c>
+      <c r="B255" t="s">
+        <v>12</v>
+      </c>
+      <c r="C255" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D255" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E255" s="7" t="s">
+        <v>1538</v>
+      </c>
+      <c r="F255" s="7" t="s">
+        <v>1539</v>
+      </c>
+      <c r="G255" s="7" t="s">
+        <v>1540</v>
+      </c>
+      <c r="H255" s="7" t="s">
+        <v>1541</v>
+      </c>
+      <c r="I255" s="7" t="s">
+        <v>1542</v>
+      </c>
+      <c r="J255" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K255" s="8" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" ht="30">
+      <c r="A256" s="3">
+        <v>255</v>
+      </c>
+      <c r="B256" t="s">
+        <v>12</v>
+      </c>
+      <c r="C256" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D256" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E256" s="7" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F256" s="7" t="s">
+        <v>1545</v>
+      </c>
+      <c r="G256" s="7" t="s">
+        <v>1546</v>
+      </c>
+      <c r="H256" s="7" t="s">
+        <v>1547</v>
+      </c>
+      <c r="I256" s="7" t="s">
+        <v>1548</v>
+      </c>
+      <c r="J256" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K256" s="8" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" ht="30">
+      <c r="A257" s="3">
+        <v>256</v>
+      </c>
+      <c r="B257" t="s">
+        <v>12</v>
+      </c>
+      <c r="C257" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D257" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E257" s="7" t="s">
+        <v>1550</v>
+      </c>
+      <c r="F257" s="7" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G257" s="7" t="s">
+        <v>1552</v>
+      </c>
+      <c r="H257" s="7" t="s">
+        <v>1553</v>
+      </c>
+      <c r="I257" s="7" t="s">
+        <v>1554</v>
+      </c>
+      <c r="J257" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K257" s="8" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" ht="30">
+      <c r="A258" s="3">
+        <v>257</v>
+      </c>
+      <c r="B258" t="s">
+        <v>12</v>
+      </c>
+      <c r="C258" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D258" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E258" s="7" t="s">
+        <v>1556</v>
+      </c>
+      <c r="F258" s="7" t="s">
+        <v>1557</v>
+      </c>
+      <c r="G258" s="7" t="s">
+        <v>1558</v>
+      </c>
+      <c r="H258" s="7" t="s">
+        <v>1559</v>
+      </c>
+      <c r="I258" s="7" t="s">
+        <v>1560</v>
+      </c>
+      <c r="J258" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K258" s="8" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" ht="60">
+      <c r="A259" s="3">
+        <v>258</v>
+      </c>
+      <c r="B259" t="s">
+        <v>12</v>
+      </c>
+      <c r="C259" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D259" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E259" s="8" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F259" s="7" t="s">
+        <v>1563</v>
+      </c>
+      <c r="G259" s="7" t="s">
+        <v>1564</v>
+      </c>
+      <c r="H259" s="7" t="s">
+        <v>1565</v>
+      </c>
+      <c r="I259" s="7" t="s">
+        <v>1566</v>
+      </c>
+      <c r="J259" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K259" s="8" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" ht="45">
+      <c r="A260" s="3">
+        <v>259</v>
+      </c>
+      <c r="B260" t="s">
+        <v>12</v>
+      </c>
+      <c r="C260" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D260" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E260" s="8" t="s">
+        <v>1568</v>
+      </c>
+      <c r="F260" s="7" t="s">
+        <v>1569</v>
+      </c>
+      <c r="G260" s="7" t="s">
+        <v>1570</v>
+      </c>
+      <c r="H260" s="7" t="s">
+        <v>1571</v>
+      </c>
+      <c r="I260" s="7" t="s">
+        <v>1572</v>
+      </c>
+      <c r="J260" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K260" s="8" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" ht="45">
+      <c r="A261" s="3">
+        <v>260</v>
+      </c>
+      <c r="B261" t="s">
+        <v>12</v>
+      </c>
+      <c r="C261" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D261" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E261" s="8" t="s">
+        <v>1574</v>
+      </c>
+      <c r="F261" s="7" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G261" s="7" t="s">
+        <v>1576</v>
+      </c>
+      <c r="H261" s="7" t="s">
+        <v>1577</v>
+      </c>
+      <c r="I261" s="7" t="s">
+        <v>1578</v>
+      </c>
+      <c r="J261" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K261" s="8" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" ht="45">
+      <c r="A262" s="3">
+        <v>261</v>
+      </c>
+      <c r="B262" t="s">
+        <v>12</v>
+      </c>
+      <c r="C262" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D262" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E262" s="8" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F262" s="7" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G262" s="7" t="s">
+        <v>1582</v>
+      </c>
+      <c r="H262" s="7" t="s">
+        <v>1583</v>
+      </c>
+      <c r="I262" s="7" t="s">
+        <v>1584</v>
+      </c>
+      <c r="J262" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K262" s="8" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" ht="45">
+      <c r="A263" s="3">
+        <v>262</v>
+      </c>
+      <c r="B263" t="s">
+        <v>12</v>
+      </c>
+      <c r="C263" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D263" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E263" s="8" t="s">
+        <v>1586</v>
+      </c>
+      <c r="F263" s="7" t="s">
+        <v>1587</v>
+      </c>
+      <c r="G263" s="7" t="s">
+        <v>1588</v>
+      </c>
+      <c r="H263" s="7" t="s">
+        <v>1589</v>
+      </c>
+      <c r="I263" s="7" t="s">
+        <v>1590</v>
+      </c>
+      <c r="J263" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K263" s="8" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" ht="45">
+      <c r="A264" s="3">
+        <v>263</v>
+      </c>
+      <c r="B264" t="s">
+        <v>12</v>
+      </c>
+      <c r="C264" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D264" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E264" s="8" t="s">
+        <v>1592</v>
+      </c>
+      <c r="F264" s="7" t="s">
+        <v>1593</v>
+      </c>
+      <c r="G264" s="7" t="s">
+        <v>1594</v>
+      </c>
+      <c r="H264" s="7" t="s">
+        <v>1595</v>
+      </c>
+      <c r="I264" s="7" t="s">
+        <v>1596</v>
+      </c>
+      <c r="J264" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K264" s="8" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" ht="45">
+      <c r="A265" s="3">
+        <v>264</v>
+      </c>
+      <c r="B265" t="s">
+        <v>12</v>
+      </c>
+      <c r="C265" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D265" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E265" s="8" t="s">
+        <v>1598</v>
+      </c>
+      <c r="F265" s="7" t="s">
+        <v>1599</v>
+      </c>
+      <c r="G265" s="7" t="s">
+        <v>1600</v>
+      </c>
+      <c r="H265" s="7" t="s">
+        <v>1601</v>
+      </c>
+      <c r="I265" s="7" t="s">
+        <v>1602</v>
+      </c>
+      <c r="J265" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K265" s="8" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" ht="30">
+      <c r="A266" s="3">
+        <v>265</v>
+      </c>
+      <c r="B266" t="s">
+        <v>12</v>
+      </c>
+      <c r="C266" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D266" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E266" s="8" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F266" s="7" t="s">
+        <v>1605</v>
+      </c>
+      <c r="G266" s="7" t="s">
+        <v>1606</v>
+      </c>
+      <c r="H266" s="7" t="s">
+        <v>1607</v>
+      </c>
+      <c r="I266" s="7" t="s">
+        <v>1608</v>
+      </c>
+      <c r="J266" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K266" s="8" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" ht="45">
+      <c r="A267" s="3">
+        <v>266</v>
+      </c>
+      <c r="B267" t="s">
+        <v>12</v>
+      </c>
+      <c r="C267" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D267" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E267" s="8" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F267" s="7" t="s">
+        <v>1611</v>
+      </c>
+      <c r="G267" s="7" t="s">
+        <v>1612</v>
+      </c>
+      <c r="H267" s="7" t="s">
+        <v>1613</v>
+      </c>
+      <c r="I267" s="7" t="s">
+        <v>1614</v>
+      </c>
+      <c r="J267" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K267" s="8" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" ht="45">
+      <c r="A268" s="3">
+        <v>267</v>
+      </c>
+      <c r="B268" t="s">
+        <v>12</v>
+      </c>
+      <c r="C268" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="D268" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E268" s="8" t="s">
+        <v>1616</v>
+      </c>
+      <c r="F268" s="7" t="s">
+        <v>1617</v>
+      </c>
+      <c r="G268" s="7" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H268" s="7" t="s">
+        <v>1619</v>
+      </c>
+      <c r="I268" s="7" t="s">
+        <v>1620</v>
+      </c>
+      <c r="J268" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K268" s="8" t="s">
+        <v>1621</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>